<commit_message>
changed template to show revenue, income, and deductibility from irs spreadsheets
</commit_message>
<xml_diff>
--- a/guidestar/data/template.xlsx
+++ b/guidestar/data/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3d5802c32daedcc/Documents/Repositories/NLP Charity Research/guidestar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_D51EEC781B57865F6F5768F44E279EF944601CFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34A5B16A-A7EE-43D3-92E0-2111E873B714}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_D51EEC781B57865F6F5768F44E279EF944601CFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0909080C-9D5A-43BD-AB17-99F279973966}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>EIN</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>Mission Statement</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Deductibility Code</t>
+  </si>
+  <si>
+    <t>Asset Code</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Income Code</t>
   </si>
 </sst>
 </file>
@@ -105,6 +120,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,10 +460,12 @@
     <col min="7" max="7" width="38.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="87.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,9 +494,24 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>